<commit_message>
Added amea thess,  updated validation for am
</commit_message>
<xml_diff>
--- a/data/amea_thes.xlsx
+++ b/data/amea_thes.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t xml:space="preserve">ΤΜΗΜΑ ΕΙΣΑΓΩΓΗΣ</t>
   </si>
@@ -167,49 +167,76 @@
     <t xml:space="preserve">454555555</t>
   </si>
   <si>
+    <t xml:space="preserve">ΑΑ988844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΒΕΓΓΟΣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΘΑΝΑΣΗΣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΜΠΑΜΠΗΣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΒΕΓΓΟΥ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΜΑΡΙΑ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27/04/2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Α</t>
+  </si>
+  <si>
+    <t xml:space="preserve">email1271011897@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thessaloniki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ελληνικη</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/07/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2024/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΕΚΕΚ ΑΜΕΑ ΘΕΣΣΑΛΟΝΙΚΗΣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THESS KEPE EKP 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΝΑΙ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">454555556</t>
+  </si>
+  <si>
     <t xml:space="preserve">ΑΑ988843</t>
   </si>
   <si>
-    <t xml:space="preserve">ΒΕΓΓΟΣ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ΘΑΝΑΣΗΣ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ΜΠΑΜΠΗΣ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ΒΕΓΓΟΥ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ΜΑΡΙΑ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27/04/2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Α</t>
-  </si>
-  <si>
-    <t xml:space="preserve">email1271011897@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">street</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thessaloniki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ελληνικη</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/07/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2024/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ΕΚΕΚ ΑΜΕΑ ΘΕΣΣΑΛΟΝΙΚΗΣ</t>
+    <t xml:space="preserve">ΜΟΥΣΤΑΚΑΣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΣΩΤΗΡΗΣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΜΟΥΣΤΑΚΑ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/07/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28/07/2022</t>
   </si>
 </sst>
 </file>
@@ -314,7 +341,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -352,6 +379,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -483,8 +514,8 @@
   </sheetPr>
   <dimension ref="A1:AQ1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG2" activeCellId="0" sqref="AG2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE3" activeCellId="0" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -496,7 +527,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="18.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.58"/>
@@ -745,8 +777,111 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>6987894565</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>2101235468</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="1" t="n">
+        <v>12345</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y3" s="2" t="n">
+        <v>12345678901</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>1234567</v>
+      </c>
+      <c r="AA3" s="2" t="n">
+        <v>24324324</v>
+      </c>
+      <c r="AB3" s="1" t="n">
+        <v>234234</v>
+      </c>
+      <c r="AC3" s="1" t="n">
+        <v>234</v>
+      </c>
+      <c r="AD3" s="1" t="n">
+        <v>2342</v>
+      </c>
+      <c r="AE3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="6"/>

</xml_diff>

<commit_message>
Added some None validations
</commit_message>
<xml_diff>
--- a/data/amea_thes.xlsx
+++ b/data/amea_thes.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t xml:space="preserve">ΤΜΗΜΑ ΕΙΣΑΓΩΓΗΣ</t>
   </si>
@@ -341,7 +341,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,10 +379,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,8 +510,8 @@
   </sheetPr>
   <dimension ref="A1:AQ1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE3" activeCellId="0" sqref="AE3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,9 +842,6 @@
       <c r="W3" s="1" t="n">
         <v>12345</v>
       </c>
-      <c r="X3" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="Y3" s="2" t="n">
         <v>12345678901</v>
       </c>
@@ -873,7 +866,7 @@
       <c r="AF3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AG3" s="9" t="s">
         <v>64</v>
       </c>
       <c r="AH3" s="2" t="s">

</xml_diff>

<commit_message>
Added saek demo, clean up
</commit_message>
<xml_diff>
--- a/data/amea_thes.xlsx
+++ b/data/amea_thes.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
   <si>
     <t xml:space="preserve">ΤΜΗΜΑ ΕΙΣΑΓΩΓΗΣ</t>
   </si>
@@ -511,7 +511,7 @@
   <dimension ref="A1:AQ1002"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X3" activeCellId="0" sqref="X3"/>
+      <selection pane="topLeft" activeCell="V3" activeCellId="1" sqref="X3 V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -842,6 +842,9 @@
       <c r="W3" s="1" t="n">
         <v>12345</v>
       </c>
+      <c r="X3" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="Y3" s="2" t="n">
         <v>12345678901</v>
       </c>

</xml_diff>